<commit_message>
1.1 update of several functions
-new sample invoice
-tweaks in existing code
-added QVC for manual packing addition, first version
</commit_message>
<xml_diff>
--- a/PL_blank.xlsx
+++ b/PL_blank.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Exa\Documents\GitHub\pdf-to-excel-Packing-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA42614-5AEC-46C6-AB19-63A93C9EF6F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5CB7B7-0A6B-492B-A3F5-32E969A42825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -490,7 +490,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -600,22 +600,8 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -623,36 +609,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -677,6 +633,30 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -688,6 +668,24 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1033,8 +1031,8 @@
   </sheetPr>
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:E17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1048,131 +1046,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="66"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="53"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="47"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="69"/>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="71"/>
+      <c r="A3" s="53"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="55"/>
     </row>
     <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="57"/>
-      <c r="B4" s="58"/>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="59"/>
+      <c r="A4" s="56"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="58"/>
     </row>
     <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="54"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="56"/>
+      <c r="A5" s="68"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="70"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="54"/>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="56"/>
+      <c r="A6" s="68"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="70"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="57"/>
-      <c r="B7" s="58"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="59"/>
+      <c r="A7" s="56"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="58"/>
     </row>
     <row r="8" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="60"/>
-      <c r="B8" s="61"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="62"/>
+      <c r="A8" s="71"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="73"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="72"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="73"/>
+      <c r="B9" s="64"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="65"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="72"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="73"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="65"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="43"/>
-      <c r="B11" s="72"/>
-      <c r="C11" s="72"/>
-      <c r="D11" s="72"/>
-      <c r="E11" s="73"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="65"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="43"/>
-      <c r="B12" s="72"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="73"/>
+      <c r="B12" s="64"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="65"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="43"/>
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="73"/>
+      <c r="B13" s="64"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="65"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="43"/>
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="73"/>
+      <c r="B14" s="64"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="65"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="43"/>
-      <c r="B15" s="72"/>
-      <c r="C15" s="72"/>
-      <c r="D15" s="72"/>
-      <c r="E15" s="73"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="65"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="43"/>
-      <c r="B16" s="72"/>
-      <c r="C16" s="72"/>
-      <c r="D16" s="72"/>
-      <c r="E16" s="73"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="65"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="44"/>
-      <c r="B17" s="74"/>
-      <c r="C17" s="74"/>
-      <c r="D17" s="74"/>
-      <c r="E17" s="75"/>
+      <c r="B17" s="66"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="67"/>
     </row>
     <row r="18" spans="1:5" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="42" t="s">
@@ -1181,10 +1179,10 @@
       <c r="B18" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="67" t="s">
+      <c r="C18" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="68"/>
+      <c r="D18" s="52"/>
       <c r="E18" s="28" t="s">
         <v>5</v>
       </c>
@@ -1309,33 +1307,33 @@
       <c r="E35" s="36"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="47"/>
-      <c r="B36" s="48"/>
+      <c r="A36" s="59"/>
+      <c r="B36" s="60"/>
       <c r="C36" s="24"/>
       <c r="D36" s="27"/>
       <c r="E36" s="29"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="49"/>
-      <c r="B37" s="48"/>
+      <c r="A37" s="61"/>
+      <c r="B37" s="60"/>
       <c r="D37" s="15"/>
       <c r="E37" s="9"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="49"/>
-      <c r="B38" s="48"/>
+      <c r="A38" s="61"/>
+      <c r="B38" s="60"/>
       <c r="D38" s="15"/>
       <c r="E38" s="9"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="49"/>
-      <c r="B39" s="48"/>
+      <c r="A39" s="61"/>
+      <c r="B39" s="60"/>
       <c r="D39" s="15"/>
       <c r="E39" s="9"/>
     </row>
     <row r="40" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="50"/>
-      <c r="B40" s="51"/>
+      <c r="A40" s="62"/>
+      <c r="B40" s="63"/>
       <c r="C40" s="7"/>
       <c r="D40" s="16"/>
       <c r="E40" s="19"/>
@@ -1380,8 +1378,8 @@
       <c r="B45" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C45" s="45"/>
-      <c r="D45" s="46"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
       <c r="E45" s="8"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -1389,8 +1387,8 @@
       <c r="B46" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C46" s="45"/>
-      <c r="D46" s="46"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
       <c r="E46" s="8"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -1412,17 +1410,15 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="8">
+    <mergeCell ref="A36:B40"/>
+    <mergeCell ref="B9:E17"/>
+    <mergeCell ref="A5:E6"/>
+    <mergeCell ref="A7:E8"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="A3:E4"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="A36:B40"/>
-    <mergeCell ref="B9:E17"/>
-    <mergeCell ref="A5:E6"/>
-    <mergeCell ref="A7:E8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
@@ -1697,15 +1693,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c026967-0f35-4eb1-b014-2813b5114173">
@@ -1714,6 +1701,15 @@
     <TaxCatchAll xmlns="43dd370b-1578-4a24-9aad-3c4e190aa6a2"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1736,14 +1732,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2842DBE6-4A40-4CFB-B426-08417731025B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5500277-CAD5-4644-8901-F56D57B117D7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1752,4 +1740,12 @@
     <ds:schemaRef ds:uri="43dd370b-1578-4a24-9aad-3c4e190aa6a2"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2842DBE6-4A40-4CFB-B426-08417731025B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
discarded specifics of the company I have used to rework the invoice to PL
</commit_message>
<xml_diff>
--- a/PL_blank.xlsx
+++ b/PL_blank.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Exa\Documents\GitHub\pdf-to-excel-Packing-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFC25AA-0755-4174-9359-05C8967411A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F15855B-731B-4DF9-83F0-85D29D9DE54B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -73,13 +73,10 @@
     <t>pcs</t>
   </si>
   <si>
-    <t>Karásek 7, BRNO,  Czech republic
-Incorporated in the Commercial Register maintained by the Regional Court in Brno, Section C, 
-Insertion 28561 
-IČ: 25504428, VAT No.: CZ25504428</t>
+    <t>Company HEADER</t>
   </si>
   <si>
-    <t>MORAVIA PROPAG s.r.o.</t>
+    <t>Company adress, VAT etc.</t>
   </si>
 </sst>
 </file>
@@ -1031,8 +1028,8 @@
   </sheetPr>
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1047,7 +1044,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="45" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="46"/>
       <c r="C1" s="46"/>
@@ -1056,7 +1053,7 @@
     </row>
     <row r="2" spans="1:5" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="71" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="72"/>
       <c r="C2" s="72"/>
@@ -1689,6 +1686,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c026967-0f35-4eb1-b014-2813b5114173">
@@ -1697,15 +1703,6 @@
     <TaxCatchAll xmlns="43dd370b-1578-4a24-9aad-3c4e190aa6a2"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1728,6 +1725,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2842DBE6-4A40-4CFB-B426-08417731025B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5500277-CAD5-4644-8901-F56D57B117D7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1736,12 +1741,4 @@
     <ds:schemaRef ds:uri="43dd370b-1578-4a24-9aad-3c4e190aa6a2"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2842DBE6-4A40-4CFB-B426-08417731025B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>